<commit_message>
Review of mappings for Wound and IllnessPerception HCIMs. Only made some cosmetic changes
</commit_message>
<xml_diff>
--- a/Mappings/IllnessPerception - STU3.xlsx
+++ b/Mappings/IllnessPerception - STU3.xlsx
@@ -1,16 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edelman\Nictiz-STU3-Zib2017\Mappings\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{321E1BB8-3E9C-4A68-B8E9-5BAAE2D7E358}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="630" windowWidth="27495" windowHeight="13995" activeTab="3"/>
+    <workbookView xWindow="630" yWindow="630" windowWidth="27495" windowHeight="13995" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="Metadata" sheetId="2" r:id="rId2"/>
     <sheet name="Information Model" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="6" r:id="rId4"/>
+    <sheet name="Research" sheetId="6" r:id="rId4"/>
     <sheet name="Data" sheetId="4" r:id="rId5"/>
     <sheet name="Terms of Use" sheetId="5" r:id="rId6"/>
   </sheets>
@@ -393,8 +399,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Calibri"/>
@@ -404,17 +410,20 @@
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -554,24 +563,27 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -709,7 +721,13 @@
     <xdr:ext cx="2856900" cy="618995"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1025" name="Picture 1"/>
+        <xdr:cNvPr id="1025" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -744,7 +762,13 @@
     <xdr:ext cx="1428750" cy="504825"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1026" name="Picture 2"/>
+        <xdr:cNvPr id="1026" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -779,7 +803,13 @@
     <xdr:ext cx="6648450" cy="3429000"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1025" name="Picture 1"/>
+        <xdr:cNvPr id="1025" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000001040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -831,11 +861,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4097"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000001100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -843,6 +876,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -872,11 +928,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4098"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -884,6 +943,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -913,11 +995,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4099"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -925,6 +1010,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -954,11 +1062,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4100"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -966,6 +1077,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -995,11 +1129,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4101"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000005100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1007,6 +1144,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1036,11 +1196,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4102"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000006100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1048,6 +1211,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1077,11 +1263,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4103"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000007100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1089,6 +1278,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1118,11 +1330,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4104"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000008100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1130,6 +1345,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1159,11 +1397,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4105"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000009100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1171,6 +1412,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1200,11 +1464,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4106"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000A100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1212,6 +1479,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1241,11 +1531,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4107"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000B100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1253,6 +1546,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1282,11 +1598,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4108"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000C100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1294,6 +1613,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1323,11 +1665,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4109"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000D100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1335,6 +1680,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1364,11 +1732,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4110"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000E100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1376,6 +1747,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1405,11 +1799,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4111"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000F100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1417,6 +1814,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1446,11 +1866,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4112"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000010100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1458,6 +1881,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1487,11 +1933,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4113"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000011100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1499,6 +1948,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1528,11 +2000,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4114"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000012100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1540,6 +2015,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1569,11 +2067,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4115"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000013100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1581,6 +2082,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1610,11 +2134,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4116"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000014100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1622,6 +2149,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1651,11 +2201,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4117"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000015100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1663,6 +2216,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1692,11 +2268,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4118"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000016100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1704,6 +2283,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1733,11 +2335,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4119"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000017100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1745,6 +2350,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1774,11 +2402,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4120"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000018100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1786,6 +2417,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1815,11 +2469,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4121"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000019100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1827,6 +2484,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1856,11 +2536,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4122"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00001A100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1868,6 +2551,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1897,11 +2603,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4123"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00001B100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1909,6 +2618,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1938,11 +2670,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4124"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00001C100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1950,6 +2685,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -1979,11 +2737,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4125"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00001D100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1991,6 +2752,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2020,11 +2804,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4126"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00001E100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -2032,6 +2819,29 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -2043,7 +2853,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2085,7 +2895,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2118,9 +2928,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2153,6 +2980,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2328,18 +3172,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="100" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2347,7 +3191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:3">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
@@ -2355,7 +3199,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
@@ -2363,7 +3207,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
@@ -2371,7 +3215,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:3">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
@@ -2379,7 +3223,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:3">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
@@ -2387,7 +3231,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="2:3">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
@@ -2395,7 +3239,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="2:3">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>14</v>
       </c>
@@ -2403,7 +3247,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="2:3">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
         <v>16</v>
       </c>
@@ -2411,7 +3255,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="2:3">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>18</v>
       </c>
@@ -2419,7 +3263,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="51">
+    <row r="12" spans="2:3" ht="51" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
         <v>55</v>
       </c>
@@ -2427,7 +3271,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="2:3" ht="25.5">
+    <row r="13" spans="2:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
         <v>57</v>
       </c>
@@ -2437,7 +3281,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C11" r:id="rId1"/>
+    <hyperlink ref="C11" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -2448,24 +3292,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="35" customWidth="1"/>
     <col min="3" max="3" width="70" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3">
-      <c r="B2" s="15" t="s">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B2" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="15"/>
-    </row>
-    <row r="3" spans="2:3">
+      <c r="C2" s="19"/>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>21</v>
       </c>
@@ -2473,7 +3317,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="2:3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>23</v>
       </c>
@@ -2481,7 +3325,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="2:3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>25</v>
       </c>
@@ -2489,7 +3333,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="2:3">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>26</v>
       </c>
@@ -2497,7 +3341,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="2:3">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>27</v>
       </c>
@@ -2505,7 +3349,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="2:3">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>28</v>
       </c>
@@ -2513,13 +3357,13 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="2:3">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="2:3">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
         <v>31</v>
       </c>
@@ -2527,13 +3371,13 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="2:3">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="2:3">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
         <v>34</v>
       </c>
@@ -2541,13 +3385,13 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="2:3">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="2:3">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
         <v>37</v>
       </c>
@@ -2555,7 +3399,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="2:3">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
         <v>39</v>
       </c>
@@ -2563,7 +3407,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="2:3">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
         <v>41</v>
       </c>
@@ -2571,7 +3415,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="2:3">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
         <v>42</v>
       </c>
@@ -2579,7 +3423,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="2:3">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
         <v>43</v>
       </c>
@@ -2587,7 +3431,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="2:3">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
         <v>45</v>
       </c>
@@ -2595,7 +3439,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="2:3">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
         <v>46</v>
       </c>
@@ -2603,7 +3447,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="2:3">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
         <v>47</v>
       </c>
@@ -2611,7 +3455,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="2:3">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B22" s="2" t="s">
         <v>49</v>
       </c>
@@ -2619,7 +3463,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="2:3">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B23" s="2" t="s">
         <v>50</v>
       </c>
@@ -2627,7 +3471,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="2:3">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B24" s="2" t="s">
         <v>52</v>
       </c>
@@ -2635,7 +3479,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="2:3">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B25" s="2" t="s">
         <v>53</v>
       </c>
@@ -2655,14 +3499,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
     </row>
   </sheetData>
@@ -2672,14 +3516,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="46.5703125" customWidth="1"/>
     <col min="3" max="3" width="47.7109375" customWidth="1"/>
@@ -2687,97 +3531,97 @@
     <col min="5" max="5" width="71.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="O1" s="16"/>
-    </row>
-    <row r="2" spans="1:15">
-      <c r="A2" s="17" t="s">
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="O1" s="15"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="E2" s="17"/>
-    </row>
-    <row r="3" spans="1:15">
-      <c r="A3" s="17" t="s">
+      <c r="E2" s="16"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="D3" s="17"/>
-    </row>
-    <row r="4" spans="1:15">
-      <c r="A4" s="17" t="s">
+      <c r="D3" s="16"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="D4" s="17"/>
-    </row>
-    <row r="5" spans="1:15">
-      <c r="A5" s="17" t="s">
+      <c r="D4" s="16"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" s="16" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
-      <c r="A6" s="17" t="s">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" s="16" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
-      <c r="A7" s="17" t="s">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" s="16" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
-      <c r="A8" s="17" t="s">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="E8" s="17"/>
-    </row>
-    <row r="9" spans="1:15">
-      <c r="A9" s="17" t="s">
+      <c r="E8" s="16"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="D9" s="18" t="s">
+      <c r="D9" s="17" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>121</v>
       </c>
       <c r="C11" t="s">
         <v>122</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="18" t="s">
         <v>120</v>
       </c>
     </row>
@@ -3455,14 +4299,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B2:T6"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="Q26" sqref="Q26"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="6" width="2" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
@@ -3478,7 +4322,7 @@
     <col min="18" max="20" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:20">
+    <row r="2" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B2" s="5" t="s">
         <v>55</v>
       </c>
@@ -3527,7 +4371,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="2:20" ht="63.75">
+    <row r="3" spans="2:20" ht="63.75" x14ac:dyDescent="0.2">
       <c r="B3" s="8" t="s">
         <v>68</v>
       </c>
@@ -3564,7 +4408,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="4" spans="2:20" ht="25.5">
+    <row r="4" spans="2:20" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B4" s="11"/>
       <c r="C4" s="12" t="s">
         <v>74</v>
@@ -3605,7 +4449,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="5" spans="2:20" ht="38.25">
+    <row r="5" spans="2:20" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B5" s="11"/>
       <c r="C5" s="12" t="s">
         <v>82</v>
@@ -3646,7 +4490,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="6" spans="2:20" ht="38.25">
+    <row r="6" spans="2:20" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B6" s="11"/>
       <c r="C6" s="12" t="s">
         <v>87</v>
@@ -3696,42 +4540,42 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B2:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="150" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="2:2" ht="140.25">
+    <row r="3" spans="2:2" ht="140.25" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="2:2">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="2:2" ht="25.5">
+    <row r="5" spans="2:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="2:2">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="7" spans="2:2" ht="38.25">
+    <row r="7" spans="2:2" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>97</v>
       </c>
@@ -3742,21 +4586,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F494F4030F39954381FEDCB9F1521453" ma:contentTypeVersion="8" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="27a32a75921fafc58b02df1cc725ea53">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c9309f2a-e493-41e5-bc1f-ce1ae85ad224" xmlns:ns3="d8b013f3-f757-4442-942f-c178d59a4411" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8dd320713f27671350e0900a33d7d303" ns2:_="" ns3:_="">
     <xsd:import namespace="c9309f2a-e493-41e5-bc1f-ce1ae85ad224"/>
@@ -3947,24 +4776,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{997170F2-B1E8-4FFA-9718-45C46AC416F1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B62DAFA-0AF0-4687-844A-215DD2C95D49}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1733C285-C2E8-4C2E-BB27-519BFB1B1C0A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3981,4 +4808,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B62DAFA-0AF0-4687-844A-215DD2C95D49}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{997170F2-B1E8-4FFA-9718-45C46AC416F1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>